<commit_message>
[t] spreadsheet.t changed utf8 test data to overlap with cp1252
</commit_message>
<xml_diff>
--- a/t/etc/data/encoding-utf8.xlsx
+++ b/t/etc/data/encoding-utf8.xlsx
@@ -19,25 +19,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Üñîçøð€</t>
+    <t>ÜñîçøðÆ</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>Elipsis…</t>
+    <t>Ellipsis…</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>ภาษาพูด</t>
+    <t>‘Single Quotes’</t>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>“Double quotes”</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -54,10 +63,6 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="IrisUPC"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,11 +85,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,9 +486,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -502,15 +508,19 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>